<commit_message>
Updated PMS_Requirements_Matrix to include promt management requirements
</commit_message>
<xml_diff>
--- a/PMS_Requirements_Matrix.xlsx
+++ b/PMS_Requirements_Matrix.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="System Requirements" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Patient Records (SUB-PR)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Clinical Workflow (SUB-CW)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Medication Mgmt (SUB-MM)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporting (SUB-RA)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Legend" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="System Requirements" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Patient Records (SUB-PR)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Clinical Workflow (SUB-CW)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Medication Mgmt (SUB-MM)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Reporting (SUB-RA)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Prompt Mgmt (SUB-PM)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Legend" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -583,7 +584,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,7 +649,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>SUB-PR-0001, SUB-CW-0001, SUB-MM-0006, SUB-RA-0004</t>
+          <t>SUB-PR-0001, SUB-CW-0001, SUB-MM-0006, SUB-RA-0004, SUB-PM-0001 (→ BE, WEB)</t>
         </is>
       </c>
     </row>
@@ -702,7 +703,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>SUB-PR-0005, SUB-CW-0004, SUB-MM-0004, SUB-RA-0003</t>
+          <t>SUB-PR-0005, SUB-CW-0004, SUB-MM-0004, SUB-RA-0003, SUB-PM-0005 (→ BE)</t>
         </is>
       </c>
     </row>
@@ -741,7 +742,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Enforce role-based access control with minimum four roles</t>
+          <t>Enforce role-based access control with minimum five roles: physician, nurse, administrator, billing, pharmacist</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -756,7 +757,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>SUB-PR-0002, SUB-CW-0002, SUB-MM-0007, SUB-RA-0005</t>
+          <t>SUB-PR-0002, SUB-CW-0002, SUB-MM-0007, SUB-RA-0005, SUB-PM-0002 (→ BE)</t>
         </is>
       </c>
     </row>
@@ -892,6 +893,33 @@
       <c r="E11" s="2" t="inlineStr">
         <is>
           <t>—</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>SYS-REQ-0011</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Provide centralized prompt management with versioning, CRUD operations, and LLM-powered comparison for all AI prompts used across the system</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0003 (→ BE, WEB), SUB-PM-0004 (→ BE, WEB), SUB-PM-0006 (→ BE, WEB), SUB-PM-0007 (→ BE, WEB, AI)</t>
         </is>
       </c>
     </row>
@@ -2323,6 +2351,283 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="55" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Domain Req</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Domain Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Backend (BE)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Web Frontend (WEB)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AI Infrastructure</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="80" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0001</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Require authenticated session for all prompt management operations</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0001-BE
+Enforce JWT auth on all prompt API endpoints via shared require_auth middleware
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0001-WEB
+Auth guard for prompt management pages using parameterized requireRole
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr"/>
+    </row>
+    <row r="3" ht="80" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0002</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Enforce RBAC: administrator can create, update, and delete prompts; administrator and physician can read prompts</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0002-BE
+Enforce role-based access control on prompt API endpoints: admin for create/update/delete, admin+physician for read
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr"/>
+    </row>
+    <row r="4" ht="80" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0003</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Support CRUD operations for prompts (name + text). Prompt names must be unique; DB unique constraint is authoritative and service layer must handle IntegrityError and return HTTP 409</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0003-BE
+REST CRUD endpoints for prompts (POST, GET, GET/{id}, PUT/{id}, DELETE/{id}). Prompt name uniqueness enforced via DB unique constraint; service catches IntegrityError and returns 409.
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0003-WEB
+Prompt CRUD forms: create form (name + text), list view, detail view, edit form. Display 409 conflict error on duplicate name.
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr"/>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0004</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Auto-versioning: every text save creates a new immutable version. Version numbers serialized via SELECT MAX(version) FOR UPDATE to prevent concurrent conflicts</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0004-BE
+Auto-versioning: on every prompt text save, insert new row into prompt_versions with auto-incremented version number. Use SELECT MAX(version) FOR UPDATE to serialize concurrent version creation. Versions are immutable once created.
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0004-WEB
+Version indicator in prompt editor: display current version number, show "saving creates new version" notice before submission
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr"/>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0005</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Log all prompt operations (create, update, delete, read, version_create, version_compare) to the audit trail with user_id, action, resource_type, resource_id, timestamp, and IP address</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0005-BE
+Audit log all prompt operations using standardized action strings: PROMPT_CREATE, PROMPT_READ, PROMPT_UPDATE, PROMPT_DELETE, VERSION_CREATE, VERSION_COMPARE. Resource type: prompt.
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr"/>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0006</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Provide paginated version history listing for each prompt (default: 20 per page, ordered by version descending)</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0006-BE
+Paginated version history API endpoint (GET /prompts/{id}/versions?page=1&amp;size=20). Returns versions ordered by version number descending with total count.
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0006-WEB
+Version history list with pagination controls for each prompt
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr"/>
+    </row>
+    <row r="8" ht="80" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>SUB-PM-0007</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>LLM-powered version comparison: given two versions of the same prompt, generate a natural-language diff summary via Anthropic Claude API. Comparison template is itself a managed prompt, bootstrapped via database migration</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0007-BE
+Version comparison API endpoint (POST /prompts/{id}/versions/compare). Accepts two version numbers, retrieves both version texts, calls Anthropic Claude API (claude-sonnet-4-20250514) with the managed comparison prompt, returns natural-language diff summary. 30-second timeout; rate-limited.
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0007-WEB
+Comparison UI: version selector (two dropdowns), trigger comparison, display natural-language diff summary returned by backend
+Status: Not Started</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>SUB-PM-0007-AI
+Anthropic Claude API integration for prompt version comparison. Uses claude-sonnet-4-20250514 model. Prompt text is NOT PHI — external API calls are acceptable. Comparison template is a managed prompt bootstrapped via migration.
+Status: Not Started</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>